<commit_message>
Ajout QuestionnaireResponse + update extensions 0293129f214352e2286fa5ae20df6c8a706dcd96
</commit_message>
<xml_diff>
--- a/299-Ajout-de-l'évaluation/ig/StructureDefinition-tddui-attachment.xlsx
+++ b/299-Ajout-de-l'évaluation/ig/StructureDefinition-tddui-attachment.xlsx
@@ -42,7 +42,7 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Pièce jointe de l’évènement</t>
+    <t>Pièce jointe</t>
   </si>
   <si>
     <t>Status</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-09-26T08:52:04+00:00</t>
+    <t>2025-09-26T11:13:08+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -81,7 +81,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Pièces jointes liées à l’événement.</t>
+    <t>Pièces jointes.</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>